<commit_message>
Added 3D Models of Kit Components
Small and Large Servo
</commit_message>
<xml_diff>
--- a/ME134_ComponentTracking.xlsx
+++ b/ME134_ComponentTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawye\OneDrive - Tufts\Tufts Classes\4 Senior\Fall\Course Assistant - ME134\ME134-Kit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A8E26B-1C31-4378-AA0F-D19CE94CC112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE3AF57-F059-436A-B97A-25BF83FE0929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="108">
   <si>
     <t>ASSET NAME</t>
   </si>
@@ -123,9 +123,6 @@
     <t>ENTER ORDERS</t>
   </si>
   <si>
-    <t>NOTES</t>
-  </si>
-  <si>
     <t>D02</t>
   </si>
   <si>
@@ -276,34 +273,103 @@
     <t>ME 134 - Demo Kit</t>
   </si>
   <si>
-    <t>Missing Two Small Servo-Motors</t>
-  </si>
-  <si>
     <t>Missing Four Small Servo-Motors</t>
   </si>
   <si>
-    <t>Stephanie</t>
-  </si>
-  <si>
-    <t>Rebecca</t>
-  </si>
-  <si>
-    <t>Taylor</t>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Checked Out</t>
+  </si>
+  <si>
+    <t>Checked In</t>
+  </si>
+  <si>
+    <t>Missing Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chris </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naizhe </t>
+  </si>
+  <si>
+    <t>Akshita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mischael </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soham </t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Sawyer</t>
+  </si>
+  <si>
+    <t>Taylor K.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Rebbeca S.</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Jared</t>
+  </si>
+  <si>
+    <t>Gus</t>
+  </si>
+  <si>
+    <t>Big Servo</t>
+  </si>
+  <si>
+    <t>Olive R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohamaed </t>
+  </si>
+  <si>
+    <t>Naizhe C.</t>
+  </si>
+  <si>
+    <t>Sawyer P.</t>
+  </si>
+  <si>
+    <t>Mischael A.</t>
+  </si>
+  <si>
+    <t>Ronan G.</t>
+  </si>
+  <si>
+    <t>Ronan O. Gissler</t>
+  </si>
+  <si>
+    <t>Mischael Anilus</t>
+  </si>
+  <si>
+    <t>Chris T.</t>
+  </si>
+  <si>
+    <t>Allison M.</t>
   </si>
   <si>
     <t>Jack A.</t>
   </si>
   <si>
-    <t>Allison Moore</t>
-  </si>
-  <si>
-    <t>Olive R.</t>
-  </si>
-  <si>
-    <t>Chris T.</t>
-  </si>
-  <si>
-    <t>Naizhe</t>
+    <t>Stephanie B.</t>
+  </si>
+  <si>
+    <t>Rebecca S.</t>
   </si>
 </sst>
 </file>
@@ -833,7 +899,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="51">
     <dxf>
       <font>
         <b val="0"/>
@@ -2200,6 +2266,12 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="dd\-mmm\-yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="dd\-mmm\-yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="dd\-mmm\-yyyy"/>
@@ -2817,16 +2889,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="T_ASSET" displayName="T_ASSET" ref="A7:E23" totalsRowShown="0" headerRowDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="T_ASSET" displayName="T_ASSET" ref="A7:E23" totalsRowShown="0" headerRowDxfId="50">
   <autoFilter ref="A7:E23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ASSET NAME"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ASSET DESCRIPTION" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="# OF ITEMS"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="RENTED OUT" dataDxfId="47">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="RENTED OUT" dataDxfId="49">
       <calculatedColumnFormula>IFERROR(SUMPRODUCT(--(T_ORDERS[ASSET]=T_ASSET[[#This Row],[ASSET NAME]]),--(T_ORDERS[RENT OUT DATE]&lt;=TD),--(T_ORDERS[RETURN DATE]&gt;=TD),T_ORDERS[QUANTITY]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IN STOCK" dataDxfId="46">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IN STOCK" dataDxfId="48">
       <calculatedColumnFormula>IFERROR((T_ASSET[[#This Row],['# OF ITEMS]]-T_ASSET[[#This Row],[RENTED OUT]]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2835,16 +2907,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="T_ORDERS" displayName="T_ORDERS" ref="A7:G23" totalsRowShown="0" headerRowDxfId="45">
-  <autoFilter ref="A7:G23" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="T_ORDERS" displayName="T_ORDERS" ref="A7:I34" totalsRowShown="0" headerRowDxfId="47">
+  <autoFilter ref="A7:I34" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ORDER NUMBER"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ORDER DATE" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ORDER DATE" dataDxfId="46"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="ASSET"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="QUANTITY"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="RENT OUT DATE" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="RETURN DATE" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="NOTES" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="RENT OUT DATE" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="RETURN DATE" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Checked Out" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{ECE72A30-B141-4AD1-A6E7-D793ED432141}" name="Checked In" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{8DEC47D6-C747-49F1-92BB-C5F5A2521ED7}" name="Missing Components" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3292,7 +3366,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3326,15 +3400,15 @@
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="52">
         <f>SUM(T_ASSET['# OF ITEMS])</f>
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D3" s="54">
         <f ca="1">SUM(T_ASSET[RENTED OUT])</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="55">
         <f ca="1">SUM(T_ASSET[IN STOCK])</f>
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="G3" s="56" t="str">
         <f ca="1">UPPER(TEXT(H3,"MMM"))</f>
@@ -3342,7 +3416,7 @@
       </c>
       <c r="H3" s="53">
         <f ca="1">TODAY()</f>
-        <v>44454</v>
+        <v>44468</v>
       </c>
       <c r="J3" s="2"/>
     </row>
@@ -3355,10 +3429,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3380,13 +3454,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="49" t="s">
-        <v>61</v>
-      </c>
       <c r="C8">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D8" s="6">
         <f ca="1">IFERROR(SUMPRODUCT(--(T_ORDERS[ASSET]=T_ASSET[[#This Row],[ASSET NAME]]),--(T_ORDERS[RENT OUT DATE]&lt;=TD),--(T_ORDERS[RETURN DATE]&gt;=TD),T_ORDERS[QUANTITY]),"")</f>
@@ -3394,12 +3468,12 @@
       </c>
       <c r="E8" s="6">
         <f ca="1">IFERROR((T_ASSET[[#This Row],['# OF ITEMS]]-T_ASSET[[#This Row],[RENTED OUT]]),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3415,7 +3489,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3431,7 +3505,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3447,7 +3521,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3463,23 +3537,23 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" s="50">
         <f ca="1">IFERROR(SUMPRODUCT(--(T_ORDERS[ASSET]=T_ASSET[[#This Row],[ASSET NAME]]),--(T_ORDERS[RENT OUT DATE]&lt;=TD),--(T_ORDERS[RETURN DATE]&gt;=TD),T_ORDERS[QUANTITY]),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="50">
         <f ca="1">IFERROR((T_ASSET[[#This Row],['# OF ITEMS]]-T_ASSET[[#This Row],[RENTED OUT]]),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3495,23 +3569,23 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" s="50">
         <f ca="1">IFERROR(SUMPRODUCT(--(T_ORDERS[ASSET]=T_ASSET[[#This Row],[ASSET NAME]]),--(T_ORDERS[RENT OUT DATE]&lt;=TD),--(T_ORDERS[RETURN DATE]&gt;=TD),T_ORDERS[QUANTITY]),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="50">
         <f ca="1">IFERROR((T_ASSET[[#This Row],['# OF ITEMS]]-T_ASSET[[#This Row],[RENTED OUT]]),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3527,7 +3601,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3543,7 +3617,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3559,29 +3633,26 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" s="50">
         <f ca="1">IFERROR(SUMPRODUCT(--(T_ORDERS[ASSET]=T_ASSET[[#This Row],[ASSET NAME]]),--(T_ORDERS[RENT OUT DATE]&lt;=TD),--(T_ORDERS[RETURN DATE]&gt;=TD),T_ORDERS[QUANTITY]),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="50">
         <f ca="1">IFERROR((T_ASSET[[#This Row],['# OF ITEMS]]-T_ASSET[[#This Row],[RENTED OUT]]),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -3597,10 +3668,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -3616,7 +3687,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3664,11 +3735,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3677,14 +3748,15 @@
     <col min="2" max="2" width="18.3984375" customWidth="1"/>
     <col min="3" max="3" width="31.265625" customWidth="1"/>
     <col min="4" max="6" width="20.73046875" customWidth="1"/>
-    <col min="7" max="7" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="38" width="4.73046875" customWidth="1"/>
+    <col min="7" max="8" width="15.59765625" customWidth="1"/>
+    <col min="9" max="9" width="21.53125" bestFit="1" customWidth="1"/>
+    <col min="10" max="38" width="4.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="25" t="s">
         <v>16</v>
       </c>
@@ -3692,10 +3764,10 @@
       <c r="D2" s="23"/>
       <c r="E2" s="48"/>
       <c r="F2" s="48" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2"/>
       <c r="C3" s="17" t="s">
         <v>21</v>
@@ -3710,40 +3782,40 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C4" s="26" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D4" s="18">
-        <v>44452</v>
+        <v>44455</v>
       </c>
       <c r="E4" s="18">
-        <v>44455</v>
+        <v>44460</v>
       </c>
       <c r="F4" s="19">
         <f>IF(I_CH_ED-I_CH_SD&gt;90,"",C_MIN_AVL)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G4" s="20" t="str">
         <f>IF(I_CH_ED-I_CH_SD&gt;90,"Please choose a window less than 90 days long","")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F5" s="24" t="str">
         <f>IF(F4&lt;0,"Not enough inventory","")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.65">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -3763,10 +3835,16 @@
         <v>10</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>77</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3774,7 +3852,7 @@
         <v>44454</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3783,13 +3861,19 @@
         <v>44454</v>
       </c>
       <c r="F8" s="4">
-        <v>44461</v>
+        <v>44463</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3797,7 +3881,7 @@
         <v>44454</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3806,13 +3890,19 @@
         <v>44454</v>
       </c>
       <c r="F9" s="4">
-        <v>44461</v>
+        <v>44463</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>3</v>
       </c>
@@ -3820,7 +3910,7 @@
         <v>44454</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3829,13 +3919,19 @@
         <v>44454</v>
       </c>
       <c r="F10" s="4">
-        <v>44461</v>
+        <v>44463</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>4</v>
       </c>
@@ -3843,7 +3939,7 @@
         <v>44454</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -3852,13 +3948,19 @@
         <v>44454</v>
       </c>
       <c r="F11" s="4">
-        <v>44461</v>
+        <v>44463</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>105</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>5</v>
       </c>
@@ -3866,7 +3968,7 @@
         <v>44454</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -3875,13 +3977,19 @@
         <v>44454</v>
       </c>
       <c r="F12" s="4">
-        <v>44461</v>
+        <v>44463</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>6</v>
       </c>
@@ -3889,7 +3997,7 @@
         <v>44454</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3898,13 +4006,19 @@
         <v>44454</v>
       </c>
       <c r="F13" s="4">
-        <v>44461</v>
+        <v>44463</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>7</v>
       </c>
@@ -3912,7 +4026,7 @@
         <v>44454</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3921,13 +4035,19 @@
         <v>44454</v>
       </c>
       <c r="F14" s="4">
-        <v>44461</v>
+        <v>44463</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+        <v>103</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>8</v>
       </c>
@@ -3935,7 +4055,7 @@
         <v>44454</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3944,64 +4064,407 @@
         <v>44454</v>
       </c>
       <c r="F15" s="4">
-        <v>44461</v>
+        <v>44463</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4">
+        <v>44454</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>44454</v>
+      </c>
+      <c r="F16" s="4">
+        <v>44463</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4">
+        <v>44454</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4">
+        <v>44454</v>
+      </c>
+      <c r="F17" s="4">
+        <v>44463</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4">
+        <v>44454</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <v>44454</v>
+      </c>
+      <c r="F18" s="4">
+        <v>44463</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>44467</v>
+      </c>
+      <c r="F20" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>44467</v>
+      </c>
+      <c r="F21" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <v>44467</v>
+      </c>
+      <c r="F22" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4">
+        <v>44467</v>
+      </c>
+      <c r="F23" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4">
+        <v>44467</v>
+      </c>
+      <c r="F24" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>17</v>
+      </c>
+      <c r="B25" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4">
+        <v>44467</v>
+      </c>
+      <c r="F25" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4">
+        <v>44467</v>
+      </c>
+      <c r="F26" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4">
+        <v>44468</v>
+      </c>
+      <c r="F27" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29" s="4">
+        <v>44467</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="4">
+        <v>44467</v>
+      </c>
+      <c r="F29" s="4">
+        <v>44481</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C8:C23" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C8:C34" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>L_ASSETS</formula1>
     </dataValidation>
   </dataValidations>
@@ -4018,7 +4481,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -4331,94 +4794,94 @@
         <v>13</v>
       </c>
       <c r="D7" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="F7" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="G7" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="H7" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="I7" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="J7" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="K7" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="L7" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="41" t="s">
+      <c r="M7" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="41" t="s">
+      <c r="N7" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="O7" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="41" t="s">
+      <c r="P7" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="41" t="s">
+      <c r="Q7" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" s="41" t="s">
+      <c r="R7" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="R7" s="41" t="s">
+      <c r="S7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="41" t="s">
+      <c r="T7" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="41" t="s">
+      <c r="U7" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="41" t="s">
+      <c r="V7" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="V7" s="41" t="s">
+      <c r="W7" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="W7" s="41" t="s">
+      <c r="X7" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="X7" s="41" t="s">
+      <c r="Y7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="Y7" s="41" t="s">
+      <c r="Z7" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="Z7" s="41" t="s">
+      <c r="AA7" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="AA7" s="41" t="s">
+      <c r="AB7" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="AB7" s="41" t="s">
+      <c r="AC7" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="AC7" s="41" t="s">
+      <c r="AD7" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="AD7" s="41" t="s">
+      <c r="AE7" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="AE7" s="41" t="s">
+      <c r="AF7" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="AF7" s="41" t="s">
+      <c r="AG7" s="41" t="s">
         <v>54</v>
-      </c>
-      <c r="AG7" s="41" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -4432,127 +4895,127 @@
       </c>
       <c r="C8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=C$6),--(T_ORDERS[RETURN DATE]&gt;=C$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=C$6),--(T_ORDERS[RETURN DATE]&gt;=C$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=D$6),--(T_ORDERS[RETURN DATE]&gt;=D$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=D$6),--(T_ORDERS[RETURN DATE]&gt;=D$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=E$6),--(T_ORDERS[RETURN DATE]&gt;=E$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=E$6),--(T_ORDERS[RETURN DATE]&gt;=E$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="F8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=F$6),--(T_ORDERS[RETURN DATE]&gt;=F$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=F$6),--(T_ORDERS[RETURN DATE]&gt;=F$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=G$6),--(T_ORDERS[RETURN DATE]&gt;=G$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=G$6),--(T_ORDERS[RETURN DATE]&gt;=G$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="H8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=H$6),--(T_ORDERS[RETURN DATE]&gt;=H$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=H$6),--(T_ORDERS[RETURN DATE]&gt;=H$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="I8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=I$6),--(T_ORDERS[RETURN DATE]&gt;=I$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=I$6),--(T_ORDERS[RETURN DATE]&gt;=I$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="J8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=J$6),--(T_ORDERS[RETURN DATE]&gt;=J$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=J$6),--(T_ORDERS[RETURN DATE]&gt;=J$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="K8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=K$6),--(T_ORDERS[RETURN DATE]&gt;=K$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=K$6),--(T_ORDERS[RETURN DATE]&gt;=K$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="L8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=L$6),--(T_ORDERS[RETURN DATE]&gt;=L$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=L$6),--(T_ORDERS[RETURN DATE]&gt;=L$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="M8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=M$6),--(T_ORDERS[RETURN DATE]&gt;=M$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=M$6),--(T_ORDERS[RETURN DATE]&gt;=M$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="N8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="O8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="P8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="Q8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=Q$6),--(T_ORDERS[RETURN DATE]&gt;=Q$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=Q$6),--(T_ORDERS[RETURN DATE]&gt;=Q$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="R8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=R$6),--(T_ORDERS[RETURN DATE]&gt;=R$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=R$6),--(T_ORDERS[RETURN DATE]&gt;=R$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="S8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="T8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="U8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="V8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="W8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="X8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="Y8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="Z8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="AA8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="AB8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="AC8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="AD8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="AE8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="AF8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="AG8" s="46">
         <f>IFERROR(IF($B8="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A8)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B8),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -4610,11 +5073,11 @@
       </c>
       <c r="N9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -4630,63 +5093,63 @@
       </c>
       <c r="S9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG9" s="47">
         <f>IFERROR(IF($B9="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A9)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B9),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -4744,11 +5207,11 @@
       </c>
       <c r="N10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -4764,63 +5227,63 @@
       </c>
       <c r="S10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10" s="47">
         <f>IFERROR(IF($B10="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A10)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B10),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -4878,11 +5341,11 @@
       </c>
       <c r="N11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -4898,63 +5361,63 @@
       </c>
       <c r="S11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG11" s="47">
         <f>IFERROR(IF($B11="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A11)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B11),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -5012,11 +5475,11 @@
       </c>
       <c r="N12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -5032,63 +5495,63 @@
       </c>
       <c r="S12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG12" s="47">
         <f>IFERROR(IF($B12="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A12)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B12),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -5114,43 +5577,43 @@
       </c>
       <c r="F13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=F$6),--(T_ORDERS[RETURN DATE]&gt;=F$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=F$6),--(T_ORDERS[RETURN DATE]&gt;=F$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=G$6),--(T_ORDERS[RETURN DATE]&gt;=G$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=G$6),--(T_ORDERS[RETURN DATE]&gt;=G$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=H$6),--(T_ORDERS[RETURN DATE]&gt;=H$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=H$6),--(T_ORDERS[RETURN DATE]&gt;=H$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=I$6),--(T_ORDERS[RETURN DATE]&gt;=I$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=I$6),--(T_ORDERS[RETURN DATE]&gt;=I$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=J$6),--(T_ORDERS[RETURN DATE]&gt;=J$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=J$6),--(T_ORDERS[RETURN DATE]&gt;=J$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=K$6),--(T_ORDERS[RETURN DATE]&gt;=K$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=K$6),--(T_ORDERS[RETURN DATE]&gt;=K$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=L$6),--(T_ORDERS[RETURN DATE]&gt;=L$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=L$6),--(T_ORDERS[RETURN DATE]&gt;=L$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=M$6),--(T_ORDERS[RETURN DATE]&gt;=M$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=M$6),--(T_ORDERS[RETURN DATE]&gt;=M$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -5166,63 +5629,63 @@
       </c>
       <c r="S13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG13" s="47">
         <f>IFERROR(IF($B13="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A13)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B13),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -5280,11 +5743,11 @@
       </c>
       <c r="N14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -5304,59 +5767,59 @@
       </c>
       <c r="T14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="47">
         <f>IFERROR(IF($B14="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A14)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B14),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -5382,43 +5845,43 @@
       </c>
       <c r="F15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=F$6),--(T_ORDERS[RETURN DATE]&gt;=F$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=F$6),--(T_ORDERS[RETURN DATE]&gt;=F$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=G$6),--(T_ORDERS[RETURN DATE]&gt;=G$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=G$6),--(T_ORDERS[RETURN DATE]&gt;=G$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=H$6),--(T_ORDERS[RETURN DATE]&gt;=H$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=H$6),--(T_ORDERS[RETURN DATE]&gt;=H$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=I$6),--(T_ORDERS[RETURN DATE]&gt;=I$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=I$6),--(T_ORDERS[RETURN DATE]&gt;=I$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=J$6),--(T_ORDERS[RETURN DATE]&gt;=J$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=J$6),--(T_ORDERS[RETURN DATE]&gt;=J$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=K$6),--(T_ORDERS[RETURN DATE]&gt;=K$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=K$6),--(T_ORDERS[RETURN DATE]&gt;=K$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=L$6),--(T_ORDERS[RETURN DATE]&gt;=L$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=L$6),--(T_ORDERS[RETURN DATE]&gt;=L$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=M$6),--(T_ORDERS[RETURN DATE]&gt;=M$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=M$6),--(T_ORDERS[RETURN DATE]&gt;=M$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -5434,63 +5897,63 @@
       </c>
       <c r="S15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG15" s="47">
         <f>IFERROR(IF($B15="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A15)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B15),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -5516,43 +5979,43 @@
       </c>
       <c r="F16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=F$6),--(T_ORDERS[RETURN DATE]&gt;=F$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=F$6),--(T_ORDERS[RETURN DATE]&gt;=F$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=G$6),--(T_ORDERS[RETURN DATE]&gt;=G$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=G$6),--(T_ORDERS[RETURN DATE]&gt;=G$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=H$6),--(T_ORDERS[RETURN DATE]&gt;=H$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=H$6),--(T_ORDERS[RETURN DATE]&gt;=H$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=I$6),--(T_ORDERS[RETURN DATE]&gt;=I$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=I$6),--(T_ORDERS[RETURN DATE]&gt;=I$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=J$6),--(T_ORDERS[RETURN DATE]&gt;=J$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=J$6),--(T_ORDERS[RETURN DATE]&gt;=J$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=K$6),--(T_ORDERS[RETURN DATE]&gt;=K$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=K$6),--(T_ORDERS[RETURN DATE]&gt;=K$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=L$6),--(T_ORDERS[RETURN DATE]&gt;=L$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=L$6),--(T_ORDERS[RETURN DATE]&gt;=L$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=M$6),--(T_ORDERS[RETURN DATE]&gt;=M$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=M$6),--(T_ORDERS[RETURN DATE]&gt;=M$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="47">
         <f>IFERROR(IF($B16="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A16)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B16),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -5682,11 +6145,11 @@
       </c>
       <c r="N17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -5702,63 +6165,63 @@
       </c>
       <c r="S17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG17" s="47">
         <f>IFERROR(IF($B17="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A17)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B17),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -5816,11 +6279,11 @@
       </c>
       <c r="N18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -5836,63 +6299,63 @@
       </c>
       <c r="S18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=S$6),--(T_ORDERS[RETURN DATE]&gt;=S$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=T$6),--(T_ORDERS[RETURN DATE]&gt;=T$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=U$6),--(T_ORDERS[RETURN DATE]&gt;=U$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=V$6),--(T_ORDERS[RETURN DATE]&gt;=V$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=W$6),--(T_ORDERS[RETURN DATE]&gt;=W$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=X$6),--(T_ORDERS[RETURN DATE]&gt;=X$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=Y$6),--(T_ORDERS[RETURN DATE]&gt;=Y$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=Z$6),--(T_ORDERS[RETURN DATE]&gt;=Z$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AA$6),--(T_ORDERS[RETURN DATE]&gt;=AA$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AB$6),--(T_ORDERS[RETURN DATE]&gt;=AB$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AC$6),--(T_ORDERS[RETURN DATE]&gt;=AC$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AD$6),--(T_ORDERS[RETURN DATE]&gt;=AD$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AE$6),--(T_ORDERS[RETURN DATE]&gt;=AE$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AF$6),--(T_ORDERS[RETURN DATE]&gt;=AF$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG18" s="47">
         <f>IFERROR(IF($B18="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A18)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B18),--(T_ORDERS[RENT OUT DATE]&lt;=AG$6),--(T_ORDERS[RETURN DATE]&gt;=AG$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="15.75" x14ac:dyDescent="0.5">
@@ -5950,11 +6413,11 @@
       </c>
       <c r="N19" s="47">
         <f>IFERROR(IF($B19="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B19),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A19)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B19),--(T_ORDERS[RENT OUT DATE]&lt;=N$6),--(T_ORDERS[RETURN DATE]&gt;=N$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" s="47">
         <f>IFERROR(IF($B19="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B19),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A19)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B19),--(T_ORDERS[RENT OUT DATE]&lt;=O$6),--(T_ORDERS[RETURN DATE]&gt;=O$6),T_ORDERS[QUANTITY]))),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19" s="47">
         <f>IFERROR(IF($B19="","",IF(I_CH_CAL=2,SUMPRODUCT(--(T_ORDERS[ASSET]=$B19),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]),INDEX(T_ASSET['# OF ITEMS], $A19)-SUMPRODUCT(--(T_ORDERS[ASSET]=$B19),--(T_ORDERS[RENT OUT DATE]&lt;=P$6),--(T_ORDERS[RETURN DATE]&gt;=P$6),T_ORDERS[QUANTITY]))),"")</f>
@@ -7887,7 +8350,7 @@
       </c>
       <c r="D3">
         <f>MIN(C4:C93)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -7896,11 +8359,11 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B35" si="0">IF(I_CH_SD+A4&gt;I_CH_ED,"",I_CH_SD+A4)</f>
-        <v>44452</v>
+        <v>44455</v>
       </c>
       <c r="C4">
         <f>IFERROR(IF(B4="","",INDEX(T_ASSET['# OF ITEMS], MATCH(I_ASSET,L_ASSETS,0))-SUMPRODUCT(--(T_ORDERS[ASSET]=I_ASSET),--(T_ORDERS[RENT OUT DATE]&lt;=B4),--(T_ORDERS[RETURN DATE]&gt;=B4),T_ORDERS[QUANTITY])),"")</f>
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -7909,11 +8372,11 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
-        <v>44453</v>
+        <v>44456</v>
       </c>
       <c r="C5">
         <f>IFERROR(IF(B5="","",INDEX(T_ASSET['# OF ITEMS], MATCH(I_ASSET,L_ASSETS,0))-SUMPRODUCT(--(T_ORDERS[ASSET]=I_ASSET),--(T_ORDERS[RENT OUT DATE]&lt;=B5),--(T_ORDERS[RETURN DATE]&gt;=B5),T_ORDERS[QUANTITY])),"")</f>
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -7922,11 +8385,11 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>44454</v>
+        <v>44457</v>
       </c>
       <c r="C6">
         <f>IFERROR(IF(B6="","",INDEX(T_ASSET['# OF ITEMS], MATCH(I_ASSET,L_ASSETS,0))-SUMPRODUCT(--(T_ORDERS[ASSET]=I_ASSET),--(T_ORDERS[RENT OUT DATE]&lt;=B6),--(T_ORDERS[RETURN DATE]&gt;=B6),T_ORDERS[QUANTITY])),"")</f>
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -7935,37 +8398,37 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>44455</v>
+        <v>44458</v>
       </c>
       <c r="C7">
         <f>IFERROR(IF(B7="","",INDEX(T_ASSET['# OF ITEMS], MATCH(I_ASSET,L_ASSETS,0))-SUMPRODUCT(--(T_ORDERS[ASSET]=I_ASSET),--(T_ORDERS[RENT OUT DATE]&lt;=B7),--(T_ORDERS[RETURN DATE]&gt;=B7),T_ORDERS[QUANTITY])),"")</f>
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="str">
+      <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C8" t="str">
+        <v>44459</v>
+      </c>
+      <c r="C8">
         <f>IFERROR(IF(B8="","",INDEX(T_ASSET['# OF ITEMS], MATCH(I_ASSET,L_ASSETS,0))-SUMPRODUCT(--(T_ORDERS[ASSET]=I_ASSET),--(T_ORDERS[RENT OUT DATE]&lt;=B8),--(T_ORDERS[RETURN DATE]&gt;=B8),T_ORDERS[QUANTITY])),"")</f>
-        <v/>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="str">
+      <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C9" t="str">
+        <v>44460</v>
+      </c>
+      <c r="C9">
         <f>IFERROR(IF(B9="","",INDEX(T_ASSET['# OF ITEMS], MATCH(I_ASSET,L_ASSETS,0))-SUMPRODUCT(--(T_ORDERS[ASSET]=I_ASSET),--(T_ORDERS[RENT OUT DATE]&lt;=B9),--(T_ORDERS[RETURN DATE]&gt;=B9),T_ORDERS[QUANTITY])),"")</f>
-        <v/>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -9063,4 +9526,292 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100756D8775A846B94481C8587225A7A1BB" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="15209ac1b3a7be222eeb0d2bc7e01628">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="605ed0c8-2bc7-4633-9157-d57951d8cd23" xmlns:ns4="7f895640-5fb6-47e0-b9c7-58c63e39d2f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f361f0745d1eef9596546bc7b4111a49" ns3:_="" ns4:_="">
+    <xsd:import namespace="605ed0c8-2bc7-4633-9157-d57951d8cd23"/>
+    <xsd:import namespace="7f895640-5fb6-47e0-b9c7-58c63e39d2f5"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="605ed0c8-2bc7-4633-9157-d57951d8cd23" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7f895640-5fb6-47e0-b9c7-58c63e39d2f5" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="14" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C45F46D7-BE44-4B0B-8965-406335D00399}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="605ed0c8-2bc7-4633-9157-d57951d8cd23"/>
+    <ds:schemaRef ds:uri="7f895640-5fb6-47e0-b9c7-58c63e39d2f5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F6EC3DE-F459-4BD9-A766-7275B3D792BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E322D-3B69-45D5-B0EA-25ADF2F9B131}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="605ed0c8-2bc7-4633-9157-d57951d8cd23"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7f895640-5fb6-47e0-b9c7-58c63e39d2f5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>